<commit_message>
using MultiVision instead of VisionThread + GoogleVision
We are no longer using multithreading. Instead, we put all images into a single request, and then send this request to Google Vision API where, with 1 API call, it reads receipt images (receipts should be present in separate image files)
TODO: implement a feature that enables the program to read multiple receipts in a single image.
</commit_message>
<xml_diff>
--- a/GoogleVision/src/tables/VergilerNewMethod.xlsx
+++ b/GoogleVision/src/tables/VergilerNewMethod.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>Tarih</t>
   </si>
@@ -129,6 +129,30 @@
   </si>
   <si>
     <t>38.00</t>
+  </si>
+  <si>
+    <t>30/07/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E ROL OFISI AS . ATAŞEHIR ŞB . MAPARK OTOPARK VE ULASIM HIZMETLERI SAN . VE TIC A.S NO : 460 </t>
+  </si>
+  <si>
+    <t>000900050006016521000192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARTH : 24/07/2022 FIS NO : 0165 2 AD x 335,00 TL / AD YENI RAKI 70 CL MIGROS PLASTIK POSET TOPKDV TOPLAM MIGROS TICARET A.S. MERKEZ SELCUK 12 IR MIGROS SATIS MGZSI ATATURK MH . KUSILAY CD . NO : 1 SELCUK / IZMIR TEL : 0 ( 85 ) 229 8094 MF FO 00053324 BUYUK MUKELLEFLER V.D.6220529513 MERKEZ ADRESI . ATATURK MAH . TURGUT OZAL BULV . NO : 7 ATASE - 13 / 1STANBUL 538121 ******* 3010 4521824 ****** 3017 ARA TOPLAM % 18 % 18 SAAT : 11 : 26 0.25 * 670 25 * 102,24 * 670,25 CRTAK POS ORTAK POS * 334,00 * 336.25 KOV TUTARI KDV Lİ TOPLAM S ASYON K NO : 0010 Z NO : 1441 MF DI 12110058 SEDIR RESTAURANT CEVAHIR ILHAN ŞİRİNCE MH . 204 SK . NO : 2 SELÇUK İZMİR 37993742150 AFİYET OLSUN TEŞEKKÜR EDERİZ 28-07-2022 SAAT : 22:24 YEMEK KDV TOP K.KARTI % 8 FIS NO : 10 TERMINAL 01922484 ( E ) ISYERI NO 0001500118 22:25 SATIS *********** 3010 LERKE ALTIPARMAK HID : AU000000041010 460,00 * 4,44 * 60,00 +60,00 Tutar : 60.00 TL KAKSILIGI MAL VEYA HİZMET ALINDI LUTFEN BU BELGEYI SAKLAYINIZ MASTERCARD KASA : KASIYER : E.BOZKUS http://www.mapark.com.tr Z No : 1093 TEŞEKKÜR EDERİZ CEK : 0053866 EKU No : 0001 MF SC 0000007733 : 30.07.2022 TARIH SAAT : 09:48 FIS NO : 0019 2 X 12,50 SIGARA BOREGI 400 G ALIŞVERİŞ POŞETİ TRAKYAESKİ KAŞAR300G ERITME PEYNİRİ 500 G L.SUZ SUT PINAR 1L 0,335 kg X 12,90 YEŞİL BİBER 0,890 kg X 12,90 DOMATES KARADENİZ EKMEĞİ SARIMSAK 250 G ODUN EKMEĞİ 5 X 4,45 SIMIT TOPKDV TOPLAM 1 ) BIM BIRLEŞIK MAĞAZALAR A.Ş Ağva Merkez Mah . Şile Cad . No : 171/1 Şile / İSTANBUL BUYUK MÜKELLEFLER </t>
+  </si>
+  <si>
+    <t>729001504362205295131750051846</t>
+  </si>
+  <si>
+    <t>3.85</t>
+  </si>
+  <si>
+    <t>2996.25</t>
+  </si>
+  <si>
+    <t>3000.10</t>
   </si>
 </sst>
 </file>
@@ -173,7 +197,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:I9"/>
+  <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -387,6 +411,32 @@
         <v>38</v>
       </c>
     </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>